<commit_message>
uardado storage todavia no bien
</commit_message>
<xml_diff>
--- a/group2 project/Database_only_interesting_columns.xlsx
+++ b/group2 project/Database_only_interesting_columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\citcea\Documents\GitHub\MUSAE\MUSAE_smart_grids\group2 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEBB77F-ACFD-4F52-A36A-9E2283BADB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8C08CF-A601-4D56-A1B6-1899A92FE827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>demand_pu</t>
   </si>
@@ -48,10 +48,19 @@
     <t>Gas_pu</t>
   </si>
   <si>
-    <t>Storage</t>
+    <t>Storage_pu</t>
   </si>
   <si>
-    <t>Storage_pu</t>
+    <t>imports</t>
+  </si>
+  <si>
+    <t>real demand</t>
+  </si>
+  <si>
+    <t>real wind</t>
+  </si>
+  <si>
+    <t>filling storage</t>
   </si>
 </sst>
 </file>
@@ -607,76 +616,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.85042710431567281</c:v>
+                  <c:v>0.32552964181478761</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70951120509192289</c:v>
+                  <c:v>0.15965386210540652</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60748437389426335</c:v>
+                  <c:v>3.6018147644945861E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5852635915077985</c:v>
+                  <c:v>-1.940902069407114E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.58176146925627958</c:v>
+                  <c:v>-3.9753721540523312E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58176146925627958</c:v>
+                  <c:v>-3.9753721540523312E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.54670995432631475</c:v>
+                  <c:v>-3.0617938406113276E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.65422616799478994</c:v>
+                  <c:v>7.8276060415353149E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.707204361530547</c:v>
+                  <c:v>0.33228168763389254</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.7231394182294224</c:v>
+                  <c:v>0.57800099861361454</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.78817979677375705</c:v>
+                  <c:v>0.69124779891805299</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.57828839107904306</c:v>
+                  <c:v>0.72291798982007438</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.41745377378621518</c:v>
+                  <c:v>0.68621429701088221</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.35214004059727949</c:v>
+                  <c:v>0.64668424257449686</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.34318995679685643</c:v>
+                  <c:v>0.63187592379946289</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.36244110834076965</c:v>
+                  <c:v>0.61847845496905629</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.3713333277334967</c:v>
+                  <c:v>0.54924839107435153</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.35944161999664942</c:v>
+                  <c:v>0.51853486777712354</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.55998503078917328</c:v>
+                  <c:v>0.59208486019698348</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.73678872593358624</c:v>
+                  <c:v>0.77565782997640054</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.89826718911456516</c:v>
+                  <c:v>0.89143216872717423</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.96423028637566632</c:v>
+                  <c:v>0.97309413416597379</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.98420339435080517</c:v>
+                  <c:v>0.81526257816838776</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1449,16 +1458,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>26670</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1481,6 +1490,50 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>335747</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>84043</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7005E92B-6C73-47BA-90CF-5CD439ECD45B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1211580" y="4701540"/>
+          <a:ext cx="5387807" cy="2568163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1684,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1695,11 +1748,12 @@
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="26" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1713,13 +1767,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="G1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0.77649586217114308</v>
       </c>
@@ -1733,15 +1798,19 @@
         <v>0.45154553050000001</v>
       </c>
       <c r="E2">
-        <f>F2/MAX($F$2:$F$25)</f>
-        <v>0.85042710431567281</v>
+        <f>F2/MIN($F$2:$F$25)</f>
+        <v>0.32552964181478761</v>
       </c>
       <c r="F2" s="6">
-        <f>A2-AVERAGE(B2:D2)</f>
-        <v>0.3125377150149431</v>
+        <f>-33.79777</f>
+        <v>-33.79777</v>
+      </c>
+      <c r="G2" s="6">
+        <f>IF(F2&lt;0,1,0)</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>0.72329460071538931</v>
       </c>
@@ -1755,15 +1824,19 @@
         <v>0.43546365910000001</v>
       </c>
       <c r="E3">
-        <f>F3/MAX($F$2:$F$25)</f>
-        <v>0.70951120509192289</v>
+        <f t="shared" ref="E3:E25" si="0">F3/MIN($F$2:$F$25)</f>
+        <v>0.15965386210540652</v>
       </c>
       <c r="F3" s="6">
-        <f>A3-AVERAGE(B3:D3)</f>
-        <v>0.26075016858189942</v>
+        <f>-16.575893</f>
+        <v>-16.575893000000001</v>
+      </c>
+      <c r="G3" s="6">
+        <f t="shared" ref="G3:G25" si="1">IF(F3&lt;0,1,0)</f>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>0.6805850106885093</v>
       </c>
@@ -1777,15 +1850,19 @@
         <v>0.43337510439999999</v>
       </c>
       <c r="E4">
-        <f>F4/MAX($F$2:$F$25)</f>
-        <v>0.60748437389426335</v>
+        <f t="shared" si="0"/>
+        <v>3.6018147644945861E-2</v>
       </c>
       <c r="F4" s="6">
-        <f>A4-AVERAGE(B4:D4)</f>
-        <v>0.22325461778052763</v>
+        <f>-3.739546</f>
+        <v>-3.7395459999999998</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>0.65783647639003529</v>
       </c>
@@ -1799,15 +1876,18 @@
         <v>0.42418546369999999</v>
       </c>
       <c r="E5">
-        <f>F5/MAX($F$2:$F$25)</f>
-        <v>0.5852635915077985</v>
+        <f t="shared" si="0"/>
+        <v>-1.940902069407114E-2</v>
       </c>
       <c r="F5" s="6">
-        <f>A5-AVERAGE(B5:D5)</f>
-        <v>0.21508832990274596</v>
+        <v>2.0151210000000002</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>0.6478929879145765</v>
       </c>
@@ -1821,15 +1901,18 @@
         <v>0.4237677527</v>
       </c>
       <c r="E6">
-        <f>F6/MAX($F$2:$F$25)</f>
-        <v>0.58176146925627958</v>
+        <f t="shared" si="0"/>
+        <v>-3.9753721540523312E-2</v>
       </c>
       <c r="F6" s="6">
-        <f>A6-AVERAGE(B6:D6)</f>
-        <v>0.21380127627917472</v>
+        <v>4.1273879999999998</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>0.6478929879145765</v>
       </c>
@@ -1843,15 +1926,18 @@
         <v>0.4237677527</v>
       </c>
       <c r="E7">
-        <f>F7/MAX($F$2:$F$25)</f>
-        <v>0.58176146925627958</v>
+        <f t="shared" si="0"/>
+        <v>-3.9753721540523312E-2</v>
       </c>
       <c r="F7" s="6">
-        <f>A7-AVERAGE(B7:D7)</f>
-        <v>0.21380127627917472</v>
+        <v>4.1273879999999998</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>0.65035451986369497</v>
       </c>
@@ -1865,15 +1951,18 @@
         <v>0.4747284879</v>
       </c>
       <c r="E8">
-        <f>F8/MAX($F$2:$F$25)</f>
-        <v>0.54670995432631475</v>
+        <f t="shared" si="0"/>
+        <v>-3.0617938406113276E-2</v>
       </c>
       <c r="F8" s="6">
-        <f>A8-AVERAGE(B8:D8)</f>
-        <v>0.20091960737606673</v>
+        <v>3.1788750000000001</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>0.68576417550320656</v>
       </c>
@@ -1887,15 +1976,18 @@
         <v>0.46971595659999998</v>
       </c>
       <c r="E9">
-        <f>F9/MAX($F$2:$F$25)</f>
-        <v>0.65422616799478994</v>
+        <f t="shared" si="0"/>
+        <v>7.8276060415353149E-2</v>
       </c>
       <c r="F9" s="6">
-        <f>A9-AVERAGE(B9:D9)</f>
-        <v>0.24043254337784598</v>
+        <v>-8.1269290000000005</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>0.77258450271974932</v>
       </c>
@@ -1909,15 +2001,18 @@
         <v>0.64766081870000003</v>
       </c>
       <c r="E10">
-        <f>F10/MAX($F$2:$F$25)</f>
-        <v>0.707204361530547</v>
+        <f t="shared" si="0"/>
+        <v>0.33228168763389254</v>
       </c>
       <c r="F10" s="6">
-        <f>A10-AVERAGE(B10:D10)</f>
-        <v>0.25990238796447718</v>
+        <v>-34.498793999999997</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>0.85466167164052753</v>
       </c>
@@ -1931,15 +2026,18 @@
         <v>0.85985797829999999</v>
       </c>
       <c r="E11">
-        <f>F11/MAX($F$2:$F$25)</f>
-        <v>0.7231394182294224</v>
+        <f t="shared" si="0"/>
+        <v>0.57800099861361454</v>
       </c>
       <c r="F11" s="6">
-        <f>A11-AVERAGE(B11:D11)</f>
-        <v>0.26575862912145165</v>
+        <v>-60.010340999999997</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>0.89337524075602681</v>
       </c>
@@ -1953,15 +2051,18 @@
         <v>0.85505430240000002</v>
       </c>
       <c r="E12">
-        <f>F12/MAX($F$2:$F$25)</f>
-        <v>0.78817979677375705</v>
+        <f t="shared" si="0"/>
+        <v>0.69124779891805299</v>
       </c>
       <c r="F12" s="6">
-        <f>A12-AVERAGE(B12:D12)</f>
-        <v>0.28966140831416165</v>
+        <v>-71.768069999999994</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>0.92327555188689225</v>
       </c>
@@ -1975,15 +2076,18 @@
         <v>0.80534670009999998</v>
       </c>
       <c r="E13">
-        <f>F13/MAX($F$2:$F$25)</f>
-        <v>0.57828839107904306</v>
+        <f t="shared" si="0"/>
+        <v>0.72291798982007438</v>
       </c>
       <c r="F13" s="6">
-        <f>A13-AVERAGE(B13:D13)</f>
-        <v>0.21252489654942086</v>
+        <v>-75.056194000000005</v>
+      </c>
+      <c r="G13" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>0.92849916396808263</v>
       </c>
@@ -1997,15 +2101,18 @@
         <v>0.67230576440000001</v>
       </c>
       <c r="E14">
-        <f>F14/MAX($F$2:$F$25)</f>
-        <v>0.41745377378621518</v>
+        <f t="shared" si="0"/>
+        <v>0.68621429701088221</v>
       </c>
       <c r="F14" s="6">
-        <f>A14-AVERAGE(B14:D14)</f>
-        <v>0.15341708645151442</v>
+        <v>-71.245472000000007</v>
+      </c>
+      <c r="G14" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>0.92096852710224997</v>
       </c>
@@ -2019,15 +2126,18 @@
         <v>0.60463659150000004</v>
       </c>
       <c r="E15">
-        <f>F15/MAX($F$2:$F$25)</f>
-        <v>0.35214004059727949</v>
+        <f t="shared" si="0"/>
+        <v>0.64668424257449686</v>
       </c>
       <c r="F15" s="6">
-        <f>A15-AVERAGE(B15:D15)</f>
-        <v>0.12941384757733521</v>
+        <v>-67.141306</v>
+      </c>
+      <c r="G15" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>0.92104048934323879</v>
       </c>
@@ -2041,15 +2151,18 @@
         <v>0.54761904760000002</v>
       </c>
       <c r="E16">
-        <f>F16/MAX($F$2:$F$25)</f>
-        <v>0.34318995679685643</v>
+        <f t="shared" si="0"/>
+        <v>0.63187592379946289</v>
       </c>
       <c r="F16" s="6">
-        <f>A16-AVERAGE(B16:D16)</f>
-        <v>0.12612463122242212</v>
+        <v>-65.603847999999999</v>
+      </c>
+      <c r="G16" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>0.92149977776366754</v>
       </c>
@@ -2063,15 +2176,18 @@
         <v>0.46825396829999999</v>
       </c>
       <c r="E17">
-        <f>F17/MAX($F$2:$F$25)</f>
-        <v>0.36244110834076965</v>
+        <f t="shared" si="0"/>
+        <v>0.61847845496905629</v>
       </c>
       <c r="F17" s="6">
-        <f>A17-AVERAGE(B17:D17)</f>
-        <v>0.13319955967238328</v>
+        <v>-64.212869999999995</v>
+      </c>
+      <c r="G17" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>0.89703896543695905</v>
       </c>
@@ -2085,15 +2201,18 @@
         <v>0.42042606519999998</v>
       </c>
       <c r="E18">
-        <f>F18/MAX($F$2:$F$25)</f>
-        <v>0.3713333277334967</v>
+        <f t="shared" si="0"/>
+        <v>0.54924839107435153</v>
       </c>
       <c r="F18" s="6">
-        <f>A18-AVERAGE(B18:D18)</f>
-        <v>0.13646751046594463</v>
+        <v>-57.025131999999999</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>0.88184858297881352</v>
       </c>
@@ -2107,15 +2226,18 @@
         <v>0.49624060149999999</v>
       </c>
       <c r="E19">
-        <f>F19/MAX($F$2:$F$25)</f>
-        <v>0.35944161999664942</v>
+        <f t="shared" si="0"/>
+        <v>0.51853486777712354</v>
       </c>
       <c r="F19" s="6">
-        <f>A19-AVERAGE(B19:D19)</f>
-        <v>0.13209722741071384</v>
+        <v>-53.836333000000003</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>0.8819607594132961</v>
       </c>
@@ -2129,15 +2251,18 @@
         <v>0.70655806180000003</v>
       </c>
       <c r="E20">
-        <f>F20/MAX($F$2:$F$25)</f>
-        <v>0.55998503078917328</v>
+        <f t="shared" si="0"/>
+        <v>0.59208486019698348</v>
       </c>
       <c r="F20" s="6">
-        <f>A20-AVERAGE(B20:D20)</f>
-        <v>0.20579828779828713</v>
+        <v>-61.472583</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>0.92154422503016065</v>
       </c>
@@ -2151,15 +2276,18 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <f>F21/MAX($F$2:$F$25)</f>
-        <v>0.73678872593358624</v>
+        <f t="shared" si="0"/>
+        <v>0.77565782997640054</v>
       </c>
       <c r="F21" s="6">
-        <f>A21-AVERAGE(B21:D21)</f>
-        <v>0.27077484205698354</v>
+        <v>-80.531852000000001</v>
+      </c>
+      <c r="G21" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>0.95986623489322065</v>
       </c>
@@ -2173,15 +2301,18 @@
         <v>0.94340016709999996</v>
       </c>
       <c r="E22">
-        <f>F22/MAX($F$2:$F$25)</f>
-        <v>0.89826718911456516</v>
+        <f t="shared" si="0"/>
+        <v>0.89143216872717423</v>
       </c>
       <c r="F22" s="6">
-        <f>A22-AVERAGE(B22:D22)</f>
-        <v>0.33011926987519002</v>
+        <v>-92.552000000000007</v>
+      </c>
+      <c r="G22" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>0.98913370161068426</v>
       </c>
@@ -2195,15 +2326,18 @@
         <v>0.93149540519999996</v>
       </c>
       <c r="E23">
-        <f>F23/MAX($F$2:$F$25)</f>
-        <v>0.96423028637566632</v>
+        <f t="shared" si="0"/>
+        <v>0.97309413416597379</v>
       </c>
       <c r="F23" s="6">
-        <f>A23-AVERAGE(B23:D23)</f>
-        <v>0.35436115443963179</v>
+        <v>-101.030467</v>
+      </c>
+      <c r="G23" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -2217,15 +2351,18 @@
         <v>0.90580618209999997</v>
       </c>
       <c r="E24">
-        <f>F24/MAX($F$2:$F$25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F24" s="6">
-        <f>A24-AVERAGE(B24:D24)</f>
-        <v>0.36750676622241241</v>
+        <v>-103.82393999999999</v>
+      </c>
+      <c r="G24" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>0.94304611933032778</v>
       </c>
@@ -2239,21 +2376,24 @@
         <v>0.73830409360000004</v>
       </c>
       <c r="E25">
-        <f>F25/MAX($F$2:$F$25)</f>
-        <v>0.98420339435080517</v>
+        <f t="shared" si="0"/>
+        <v>0.81526257816838776</v>
       </c>
       <c r="F25" s="6">
-        <f>A25-AVERAGE(B25:D25)</f>
-        <v>0.36170140676298612</v>
+        <v>-84.643772999999996</v>
+      </c>
+      <c r="G25" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
final thing, still extra lines missing
</commit_message>
<xml_diff>
--- a/group2 project/Database_only_interesting_columns.xlsx
+++ b/group2 project/Database_only_interesting_columns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\citcea\Documents\GitHub\MUSAE\MUSAE_smart_grids\group2 project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8C08CF-A601-4D56-A1B6-1899A92FE827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8217C2D-C503-4645-80CD-E535A7A5BBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1455" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>demand_pu</t>
   </si>
@@ -51,16 +51,10 @@
     <t>Storage_pu</t>
   </si>
   <si>
-    <t>imports</t>
+    <t>storage level</t>
   </si>
   <si>
-    <t>real demand</t>
-  </si>
-  <si>
-    <t>real wind</t>
-  </si>
-  <si>
-    <t>filling storage</t>
+    <t>Storage</t>
   </si>
 </sst>
 </file>
@@ -197,11 +191,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Power generation</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> pu</a:t>
+              <a:t>Generation curves</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -351,7 +341,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BB32-434D-A671-028F8CD56732}"/>
+              <c16:uniqueId val="{00000000-EA29-4FE1-8C56-D210675194BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -465,7 +455,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BB32-434D-A671-028F8CD56732}"/>
+              <c16:uniqueId val="{00000001-EA29-4FE1-8C56-D210675194BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -579,7 +569,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BB32-434D-A671-028F8CD56732}"/>
+              <c16:uniqueId val="{00000002-EA29-4FE1-8C56-D210675194BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -616,76 +606,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>0.32552964181478761</c:v>
+                  <c:v>0.66666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15965386210540652</c:v>
+                  <c:v>0.66666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6018147644945861E-2</c:v>
+                  <c:v>-0.33333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.940902069407114E-2</c:v>
+                  <c:v>-0.66666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.9753721540523312E-2</c:v>
+                  <c:v>-0.66666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.9753721540523312E-2</c:v>
+                  <c:v>0.33333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.0617938406113276E-2</c:v>
+                  <c:v>0.66666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.8276060415353149E-2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.33228168763389254</c:v>
+                  <c:v>0.66666666666666674</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57800099861361454</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.69124779891805299</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.72291798982007438</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.68621429701088221</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.64668424257449686</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63187592379946289</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.61847845496905629</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.54924839107435153</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.51853486777712354</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.59208486019698348</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.77565782997640054</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.89143216872717423</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.97309413416597379</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.81526257816838776</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -693,7 +683,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-BB32-434D-A671-028F8CD56732}"/>
+              <c16:uniqueId val="{00000003-EA29-4FE1-8C56-D210675194BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -706,11 +696,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2034096015"/>
-        <c:axId val="2034100591"/>
+        <c:axId val="739534767"/>
+        <c:axId val="739537263"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2034096015"/>
+        <c:axId val="739534767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2034100591"/>
+        <c:crossAx val="739537263"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -760,7 +750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2034100591"/>
+        <c:axId val="739537263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +801,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2034096015"/>
+        <c:crossAx val="739534767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1456,54 +1446,18 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{524031E2-27C0-4907-B3E3-84C197B4D5BE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>335747</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>84043</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285264</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133573</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1519,21 +1473,57 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1211580" y="4701540"/>
-          <a:ext cx="5387807" cy="2568163"/>
+          <a:off x="4743450" y="4810125"/>
+          <a:ext cx="5382092" cy="2524348"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>654843</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>18455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>446484</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>168236</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A69ADC9B-79B3-491F-AB3D-ECA712F142BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1739,16 +1729,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I3" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -1773,14 +1763,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
@@ -1798,16 +1784,14 @@
         <v>0.45154553050000001</v>
       </c>
       <c r="E2">
-        <f>F2/MIN($F$2:$F$25)</f>
-        <v>0.32552964181478761</v>
+        <f>G2/MIN($G$2:$G$25)</f>
+        <v>0.66666666666666674</v>
       </c>
       <c r="F2" s="6">
-        <f>-33.79777</f>
-        <v>-33.79777</v>
-      </c>
-      <c r="G2" s="6">
-        <f>IF(F2&lt;0,1,0)</f>
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>-0.2</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1824,16 +1808,15 @@
         <v>0.43546365910000001</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E25" si="0">F3/MIN($F$2:$F$25)</f>
-        <v>0.15965386210540652</v>
+        <f t="shared" ref="E3:E25" si="0">G3/MIN($G$2:$G$25)</f>
+        <v>0.66666666666666674</v>
       </c>
       <c r="F3" s="6">
-        <f>-16.575893</f>
-        <v>-16.575893000000001</v>
-      </c>
-      <c r="G3" s="6">
-        <f t="shared" ref="G3:G25" si="1">IF(F3&lt;0,1,0)</f>
-        <v>1</v>
+        <f>F2+G3</f>
+        <v>0.3</v>
+      </c>
+      <c r="G3">
+        <v>-0.2</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1851,15 +1834,14 @@
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>3.6018147644945861E-2</v>
+        <v>-0.33333333333333337</v>
       </c>
       <c r="F4" s="6">
-        <f>-3.739546</f>
-        <v>-3.7395459999999998</v>
-      </c>
-      <c r="G4" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F3+G4</f>
+        <v>0.4</v>
+      </c>
+      <c r="G4">
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1877,14 +1859,14 @@
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>-1.940902069407114E-2</v>
+        <v>-0.66666666666666674</v>
       </c>
       <c r="F5" s="6">
-        <v>2.0151210000000002</v>
-      </c>
-      <c r="G5" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F4+G5</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G5">
+        <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1902,14 +1884,14 @@
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>-3.9753721540523312E-2</v>
+        <v>-0.66666666666666674</v>
       </c>
       <c r="F6" s="6">
-        <v>4.1273879999999998</v>
-      </c>
-      <c r="G6" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F5+G6</f>
+        <v>0.8</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1927,14 +1909,14 @@
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>-3.9753721540523312E-2</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="F7" s="6">
-        <v>4.1273879999999998</v>
-      </c>
-      <c r="G7" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F6+G7</f>
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="G7">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1952,14 +1934,14 @@
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>-3.0617938406113276E-2</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="F8" s="6">
-        <v>3.1788750000000001</v>
-      </c>
-      <c r="G8" s="6">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>F7+G8</f>
+        <v>0.5</v>
+      </c>
+      <c r="G8">
+        <v>-0.2</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1977,14 +1959,14 @@
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>7.8276060415353149E-2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="6">
-        <v>-8.1269290000000005</v>
-      </c>
-      <c r="G9" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F8+G9</f>
+        <v>0.2</v>
+      </c>
+      <c r="G9">
+        <v>-0.3</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2002,14 +1984,14 @@
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>0.33228168763389254</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="F10" s="6">
-        <v>-34.498793999999997</v>
-      </c>
-      <c r="G10" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F9+G10</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>-0.2</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2027,14 +2009,14 @@
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>0.57800099861361454</v>
+        <v>0</v>
       </c>
       <c r="F11" s="6">
-        <v>-60.010340999999997</v>
-      </c>
-      <c r="G11" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F10+G11</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2052,14 +2034,14 @@
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>0.69124779891805299</v>
+        <v>0</v>
       </c>
       <c r="F12" s="6">
-        <v>-71.768069999999994</v>
-      </c>
-      <c r="G12" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F11+G12</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2077,14 +2059,14 @@
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0.72291798982007438</v>
+        <v>0</v>
       </c>
       <c r="F13" s="6">
-        <v>-75.056194000000005</v>
-      </c>
-      <c r="G13" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F12+G13</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2102,14 +2084,14 @@
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>0.68621429701088221</v>
+        <v>0</v>
       </c>
       <c r="F14" s="6">
-        <v>-71.245472000000007</v>
-      </c>
-      <c r="G14" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F13+G14</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2127,14 +2109,14 @@
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0.64668424257449686</v>
+        <v>0</v>
       </c>
       <c r="F15" s="6">
-        <v>-67.141306</v>
-      </c>
-      <c r="G15" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F14+G15</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2152,14 +2134,14 @@
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>0.63187592379946289</v>
+        <v>0</v>
       </c>
       <c r="F16" s="6">
-        <v>-65.603847999999999</v>
-      </c>
-      <c r="G16" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F15+G16</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2177,14 +2159,14 @@
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>0.61847845496905629</v>
+        <v>0</v>
       </c>
       <c r="F17" s="6">
-        <v>-64.212869999999995</v>
-      </c>
-      <c r="G17" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F16+G17</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2202,14 +2184,14 @@
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>0.54924839107435153</v>
+        <v>0</v>
       </c>
       <c r="F18" s="6">
-        <v>-57.025131999999999</v>
-      </c>
-      <c r="G18" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F17+G18</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2227,14 +2209,14 @@
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>0.51853486777712354</v>
+        <v>0</v>
       </c>
       <c r="F19" s="6">
-        <v>-53.836333000000003</v>
-      </c>
-      <c r="G19" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F18+G19</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2252,14 +2234,14 @@
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>0.59208486019698348</v>
+        <v>0</v>
       </c>
       <c r="F20" s="6">
-        <v>-61.472583</v>
-      </c>
-      <c r="G20" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F19+G20</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2277,14 +2259,14 @@
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>0.77565782997640054</v>
+        <v>0</v>
       </c>
       <c r="F21" s="6">
-        <v>-80.531852000000001</v>
-      </c>
-      <c r="G21" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F20+G21</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2302,14 +2284,14 @@
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>0.89143216872717423</v>
+        <v>0</v>
       </c>
       <c r="F22" s="6">
-        <v>-92.552000000000007</v>
-      </c>
-      <c r="G22" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F21+G22</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2327,14 +2309,14 @@
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>0.97309413416597379</v>
+        <v>0</v>
       </c>
       <c r="F23" s="6">
-        <v>-101.030467</v>
-      </c>
-      <c r="G23" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F22+G23</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2352,14 +2334,14 @@
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="6">
-        <v>-103.82393999999999</v>
-      </c>
-      <c r="G24" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F23+G24</f>
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2377,14 +2359,14 @@
       </c>
       <c r="E25">
         <f t="shared" si="0"/>
-        <v>0.81526257816838776</v>
+        <v>0</v>
       </c>
       <c r="F25" s="6">
-        <v>-84.643772999999996</v>
-      </c>
-      <c r="G25" s="6">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>F24+G25</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>